<commit_message>
updated edit photos screen
</commit_message>
<xml_diff>
--- a/doc/dds_workbook.xlsx
+++ b/doc/dds_workbook.xlsx
@@ -11,6 +11,7 @@
     <sheet name="rights" sheetId="2" r:id="rId2"/>
     <sheet name="grants" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="photos" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="87">
   <si>
     <t>teasers</t>
   </si>
@@ -180,7 +181,109 @@
     <t>Video Gallery [show]</t>
   </si>
   <si>
-    <t>photographer</t>
+    <t>GTU_Eggdrop_2012_01.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_02.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_03.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_04.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_05.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_06.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_07.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_08.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_09.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_10.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_11.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_12.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_13.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_14.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_15.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_16.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_17.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_18.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_19.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_20.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_21.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_22.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_23.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_24.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_25.jpg</t>
+  </si>
+  <si>
+    <t>GTU_Eggdrop_2012_26.jpg</t>
+  </si>
+  <si>
+    <t>gallery_id</t>
+  </si>
+  <si>
+    <t>photographer_id</t>
+  </si>
+  <si>
+    <t>photo_title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>photographer: role id = 4</t>
   </si>
 </sst>
 </file>
@@ -265,8 +368,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -348,7 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -384,6 +497,11 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -419,6 +537,11 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4462,10 +4585,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4480,7 +4603,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4573,100 +4696,100 @@
     </row>
     <row r="12" spans="1:4">
       <c r="B12">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
       <c r="D15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="B16">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="6">
+    <row r="21" spans="2:4">
+      <c r="B21" s="6">
         <v>46</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="6">
+      <c r="D21" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="6">
         <v>49</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="6">
+    <row r="23" spans="2:4">
+      <c r="B23" s="6">
         <v>47</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="6">
+    <row r="24" spans="2:4">
+      <c r="B24" s="6">
         <v>48</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4678,4 +4801,375 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'"&amp;F2&amp;"','"&amp;G2&amp;"','2012-03-30','2012-03030','2012_egg_drop');"</f>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_01.jpg','1','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K27" si="0">"INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'"&amp;F3&amp;"','"&amp;G3&amp;"','2012-03-30','2012-03030','2012_egg_drop');"</f>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_02.jpg','2','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_03.jpg','3','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_04.jpg','4','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_05.jpg','5','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_06.jpg','6','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_07.jpg','7','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_08.jpg','8','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_09.jpg','9','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_10.jpg','10','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_11.jpg','11','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_12.jpg','12','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_13.jpg','13','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_14.jpg','14','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_15.jpg','15','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11">
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_16.jpg','16','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11">
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_17.jpg','17','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="19" spans="6:11">
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_18.jpg','18','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11">
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_19.jpg','19','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11">
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_20.jpg','20','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11">
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_21.jpg','21','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11">
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_22.jpg','22','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11">
+      <c r="F24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_23.jpg','23','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="25" spans="6:11">
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_24.jpg','24','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="26" spans="6:11">
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_25.jpg','25','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11">
+      <c r="F27" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_26.jpg','26','2012-03-30','2012-03030','2012_egg_drop');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added airsho 2011 photos
</commit_message>
<xml_diff>
--- a/doc/dds_workbook.xlsx
+++ b/doc/dds_workbook.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pages Sidebars" sheetId="1" r:id="rId1"/>
     <sheet name="rights" sheetId="2" r:id="rId2"/>
     <sheet name="grants" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="roles" sheetId="4" r:id="rId4"/>
     <sheet name="photos" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="129">
   <si>
     <t>teasers</t>
   </si>
@@ -284,6 +284,132 @@
   </si>
   <si>
     <t>photographer: role id = 4</t>
+  </si>
+  <si>
+    <t>member: role_id = 5</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_01.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_02.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_03.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_04.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_05.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_06.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_07.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_08.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_09.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_10.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_11.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_12.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_13.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_14.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_15.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_16.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_17.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_18.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_19.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_20.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_21.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_22.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_23.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_24.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_25.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_26.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_27.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_28.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_29.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_30.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_31.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_32.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_33.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_34.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_35.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_36.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_37.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_38.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_39.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_40.jpg</t>
+  </si>
+  <si>
+    <t>Annual_Repairs_Etc_2012_41.jpg</t>
   </si>
 </sst>
 </file>
@@ -368,8 +494,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -461,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -502,6 +672,28 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -542,6 +734,28 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -990,10 +1204,10 @@
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A58" sqref="A58:C61"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2981,10 +3195,10 @@
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C67" sqref="C67:C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4585,10 +4799,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4596,17 +4810,17 @@
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="B4" s="6">
         <v>22</v>
       </c>
@@ -4616,8 +4830,12 @@
       <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" t="str">
+        <f>"INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES ("&amp;B4&amp;",4,'2012-05-22','2012-05-22');"</f>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (22,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="B5" s="6">
         <v>62</v>
       </c>
@@ -4627,8 +4845,12 @@
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F15" si="0">"INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES ("&amp;B5&amp;",4,'2012-05-22','2012-05-22');"</f>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (62,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="B6" s="6">
         <v>23</v>
       </c>
@@ -4638,8 +4860,12 @@
       <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (23,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="B7" s="6">
         <v>24</v>
       </c>
@@ -4649,8 +4875,12 @@
       <c r="D7" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (24,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8">
         <v>63</v>
       </c>
@@ -4660,8 +4890,12 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (63,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="B9">
         <v>66</v>
       </c>
@@ -4671,8 +4905,12 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (66,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10">
         <v>64</v>
       </c>
@@ -4682,8 +4920,12 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (64,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="B11">
         <v>65</v>
       </c>
@@ -4693,8 +4935,12 @@
       <c r="D11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (65,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="B12">
         <v>74</v>
       </c>
@@ -4704,8 +4950,12 @@
       <c r="D12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (74,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="B13">
         <v>77</v>
       </c>
@@ -4715,8 +4965,12 @@
       <c r="D13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (77,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="B14">
         <v>76</v>
       </c>
@@ -4726,8 +4980,12 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (76,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="B15">
         <v>75</v>
       </c>
@@ -4737,19 +4995,17 @@
       <c r="D15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (75,4,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="B21" s="6">
         <v>46</v>
       </c>
@@ -4759,8 +5015,12 @@
       <c r="D21" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:4">
+      <c r="F21" t="str">
+        <f>"INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES ("&amp;B21&amp;",5,'2012-05-22','2012-05-22');"</f>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (46,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="B22" s="6">
         <v>49</v>
       </c>
@@ -4770,8 +5030,12 @@
       <c r="D22" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:4">
+      <c r="F22" t="str">
+        <f t="shared" ref="F22:F29" si="1">"INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES ("&amp;B22&amp;",5,'2012-05-22','2012-05-22');"</f>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (49,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="B23" s="6">
         <v>47</v>
       </c>
@@ -4781,8 +5045,12 @@
       <c r="D23" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="2:4">
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (47,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="B24" s="6">
         <v>48</v>
       </c>
@@ -4792,9 +5060,89 @@
       <c r="D24" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (48,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (92,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (91,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (25,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (26,5,'2012-05-22','2012-05-22');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `grants` (`right_id`,`role_id`,`created_at`,`updated_at`) VALUES (28,5,'2012-05-22','2012-05-22');</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4805,10 +5153,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K27"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5163,6 +5514,498 @@
         <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (14,9,'GTU_Eggdrop_2012_26.jpg','26','2012-03-30','2012-03030','2012_egg_drop');</v>
       </c>
     </row>
+    <row r="30" spans="6:11">
+      <c r="F30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="str">
+        <f>"INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'"&amp;F30&amp;"','"&amp;G30&amp;"','2012-02-28','2012-02-28','2012_maintenance');"</f>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_01.jpg','1','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="31" spans="6:11">
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" ref="K31:K70" si="1">"INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'"&amp;F31&amp;"','"&amp;G31&amp;"','2012-02-28','2012-02-28','2012_maintenance');"</f>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_02.jpg','2','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="32" spans="6:11">
+      <c r="F32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_03.jpg','3','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="33" spans="6:11">
+      <c r="F33" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_04.jpg','4','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11">
+      <c r="F34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_05.jpg','5','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="35" spans="6:11">
+      <c r="F35" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_06.jpg','6','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11">
+      <c r="F36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_07.jpg','7','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11">
+      <c r="F37" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37">
+        <v>8</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_08.jpg','8','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11">
+      <c r="F38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38">
+        <v>9</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_09.jpg','9','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11">
+      <c r="F39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39">
+        <v>10</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_10.jpg','10','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11">
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40">
+        <v>11</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_11.jpg','11','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11">
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41">
+        <v>12</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_12.jpg','12','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11">
+      <c r="F42" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42">
+        <v>13</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_13.jpg','13','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11">
+      <c r="F43" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43">
+        <v>14</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_14.jpg','14','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11">
+      <c r="F44" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44">
+        <v>15</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_15.jpg','15','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11">
+      <c r="F45" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45">
+        <v>16</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_16.jpg','16','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11">
+      <c r="F46" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46">
+        <v>17</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_17.jpg','17','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="47" spans="6:11">
+      <c r="F47" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47">
+        <v>18</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_18.jpg','18','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="48" spans="6:11">
+      <c r="F48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G48">
+        <v>19</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_19.jpg','19','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="49" spans="6:11">
+      <c r="F49" t="s">
+        <v>107</v>
+      </c>
+      <c r="G49">
+        <v>20</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_20.jpg','20','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11">
+      <c r="F50" t="s">
+        <v>108</v>
+      </c>
+      <c r="G50">
+        <v>21</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_21.jpg','21','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="51" spans="6:11">
+      <c r="F51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51">
+        <v>22</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_22.jpg','22','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11">
+      <c r="F52" t="s">
+        <v>110</v>
+      </c>
+      <c r="G52">
+        <v>23</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_23.jpg','23','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11">
+      <c r="F53" t="s">
+        <v>111</v>
+      </c>
+      <c r="G53">
+        <v>24</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_24.jpg','24','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11">
+      <c r="F54" t="s">
+        <v>112</v>
+      </c>
+      <c r="G54">
+        <v>25</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_25.jpg','25','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11">
+      <c r="F55" t="s">
+        <v>113</v>
+      </c>
+      <c r="G55">
+        <v>26</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_26.jpg','26','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11">
+      <c r="F56" t="s">
+        <v>114</v>
+      </c>
+      <c r="G56">
+        <v>27</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_27.jpg','27','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11">
+      <c r="F57" t="s">
+        <v>115</v>
+      </c>
+      <c r="G57">
+        <v>28</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_28.jpg','28','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11">
+      <c r="F58" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58">
+        <v>29</v>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_29.jpg','29','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11">
+      <c r="F59" t="s">
+        <v>117</v>
+      </c>
+      <c r="G59">
+        <v>30</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_30.jpg','30','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11">
+      <c r="F60" t="s">
+        <v>118</v>
+      </c>
+      <c r="G60">
+        <v>31</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_31.jpg','31','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11">
+      <c r="F61" t="s">
+        <v>119</v>
+      </c>
+      <c r="G61">
+        <v>32</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_32.jpg','32','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11">
+      <c r="F62" t="s">
+        <v>120</v>
+      </c>
+      <c r="G62">
+        <v>33</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_33.jpg','33','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="63" spans="6:11">
+      <c r="F63" t="s">
+        <v>121</v>
+      </c>
+      <c r="G63">
+        <v>34</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_34.jpg','34','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="64" spans="6:11">
+      <c r="F64" t="s">
+        <v>122</v>
+      </c>
+      <c r="G64">
+        <v>35</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_35.jpg','35','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="65" spans="6:11">
+      <c r="F65" t="s">
+        <v>123</v>
+      </c>
+      <c r="G65">
+        <v>36</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_36.jpg','36','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="66" spans="6:11">
+      <c r="F66" t="s">
+        <v>124</v>
+      </c>
+      <c r="G66">
+        <v>37</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_37.jpg','37','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="67" spans="6:11">
+      <c r="F67" t="s">
+        <v>125</v>
+      </c>
+      <c r="G67">
+        <v>38</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_38.jpg','38','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="68" spans="6:11">
+      <c r="F68" t="s">
+        <v>126</v>
+      </c>
+      <c r="G68">
+        <v>39</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_39.jpg','39','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="69" spans="6:11">
+      <c r="F69" t="s">
+        <v>127</v>
+      </c>
+      <c r="G69">
+        <v>40</v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_40.jpg','40','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
+    <row r="70" spans="6:11">
+      <c r="F70" t="s">
+        <v>128</v>
+      </c>
+      <c r="G70">
+        <v>41</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `photos` (`gallery_id`,`photographer_id`,`filename`,`order`,`created_at`,`updated_at`,`path`) VALUES (15,9,'Annual_Repairs_Etc_2012_41.jpg','41','2012-02-28','2012-02-28','2012_maintenance');</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>